<commit_message>
Prototype 2.1.1 Refinement - Content Update 201026a - Content Update 201026b - Content Update 201027a - Content Update 201031a - LSTM Model and Content Update 201031a
</commit_message>
<xml_diff>
--- a/data/result_history/_training_report.xlsx
+++ b/data/result_history/_training_report.xlsx
@@ -1,17 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+  <si>
+    <t>epoch</t>
+  </si>
+  <si>
+    <t>loss</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -54,86 +68,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -426,7 +372,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,24 +380,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>epoch</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>loss</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>accuracy</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
@@ -459,13 +399,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>68.01267266273499</v>
+        <v>65.15364050865173</v>
       </c>
       <c r="D2" t="n">
-        <v>57.43032693862915</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>64.5531177520752</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
@@ -473,13 +413,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>61.10079288482666</v>
+        <v>43.45792829990387</v>
       </c>
       <c r="D3" t="n">
-        <v>65.02391695976257</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>80.9173047542572</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
@@ -487,13 +427,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>53.18518280982971</v>
+        <v>33.17215144634247</v>
       </c>
       <c r="D4" t="n">
-        <v>75.23729801177979</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>85.89110970497131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
@@ -501,13 +441,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>40.70965349674225</v>
+        <v>29.88094985485077</v>
       </c>
       <c r="D5" t="n">
-        <v>81.97281360626221</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>87.30351328849792</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
@@ -515,13 +455,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>34.61340963840485</v>
+        <v>28.05566787719727</v>
       </c>
       <c r="D6" t="n">
-        <v>85.3975236415863</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>88.3134663105011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
@@ -529,13 +469,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>31.61840438842773</v>
+        <v>26.72634720802307</v>
       </c>
       <c r="D7" t="n">
-        <v>86.54415607452393</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>88.95891904830933</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
@@ -543,13 +483,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>29.85914051532745</v>
+        <v>25.58122575283051</v>
       </c>
       <c r="D8" t="n">
-        <v>87.44779229164124</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>89.54362273216248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
@@ -557,13 +497,13 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>28.44698131084442</v>
+        <v>24.7805193066597</v>
       </c>
       <c r="D9" t="n">
-        <v>88.04009556770325</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>90.08277058601379</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
@@ -571,13 +511,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>27.34716832637787</v>
+        <v>23.48838597536087</v>
       </c>
       <c r="D10" t="n">
-        <v>88.73111009597778</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>90.51560759544373</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
@@ -585,153 +525,13 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>26.50557458400726</v>
+        <v>22.30526506900787</v>
       </c>
       <c r="D11" t="n">
-        <v>89.0196681022644</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>11</v>
-      </c>
-      <c r="C12" t="n">
-        <v>25.84653794765472</v>
-      </c>
-      <c r="D12" t="n">
-        <v>89.1715407371521</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>12</v>
-      </c>
-      <c r="C13" t="n">
-        <v>24.96126145124435</v>
-      </c>
-      <c r="D13" t="n">
-        <v>89.75624442100525</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>13</v>
-      </c>
-      <c r="C14" t="n">
-        <v>24.41578656435013</v>
-      </c>
-      <c r="D14" t="n">
-        <v>89.96886610984802</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
-        <v>14</v>
-      </c>
-      <c r="C15" t="n">
-        <v>24.41580444574356</v>
-      </c>
-      <c r="D15" t="n">
-        <v>90.05239605903625</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
-        <v>15</v>
-      </c>
-      <c r="C16" t="n">
-        <v>23.71015399694443</v>
-      </c>
-      <c r="D16" t="n">
-        <v>90.27261137962341</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>16</v>
-      </c>
-      <c r="C17" t="n">
-        <v>22.9899138212204</v>
-      </c>
-      <c r="D17" t="n">
-        <v>90.50801396369934</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="n">
-        <v>17</v>
-      </c>
-      <c r="C18" t="n">
-        <v>22.68020957708359</v>
-      </c>
-      <c r="D18" t="n">
-        <v>90.76619148254395</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>18</v>
-      </c>
-      <c r="C19" t="n">
-        <v>21.6458648443222</v>
-      </c>
-      <c r="D19" t="n">
-        <v>91.3888692855835</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>19</v>
-      </c>
-      <c r="C20" t="n">
-        <v>20.65567076206207</v>
-      </c>
-      <c r="D20" t="n">
-        <v>91.56352281570435</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>20</v>
-      </c>
-      <c r="C21" t="n">
-        <v>20.80679088830948</v>
-      </c>
-      <c r="D21" t="n">
-        <v>91.85207486152649</v>
+        <v>90.89528322219849</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Prototype 2.3.1 Improvement - LSTM Model Update 201118a - LSTM Model & Content Update 201119a - Content Update 201119b - Preprocessing & LSTM Model Update 201123 - Add debugging code and some updates 201124 - Some cleaning 201125 - Content Update 201126a - System Update 201220a
</commit_message>
<xml_diff>
--- a/data/result_history/_training_report.xlsx
+++ b/data/result_history/_training_report.xlsx
@@ -372,7 +372,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -399,10 +399,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>65.15364050865173</v>
+        <v>0.6793167591094971</v>
       </c>
       <c r="D2" t="n">
-        <v>64.5531177520752</v>
+        <v>0.5790757536888123</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -413,10 +413,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>43.45792829990387</v>
+        <v>0.6305791735649109</v>
       </c>
       <c r="D3" t="n">
-        <v>80.9173047542572</v>
+        <v>0.6393302083015442</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -427,10 +427,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>33.17215144634247</v>
+        <v>0.5334708094596863</v>
       </c>
       <c r="D4" t="n">
-        <v>85.89110970497131</v>
+        <v>0.7329421639442444</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -441,10 +441,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>29.88094985485077</v>
+        <v>0.4828438460826874</v>
       </c>
       <c r="D5" t="n">
-        <v>87.30351328849792</v>
+        <v>0.7683433294296265</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -455,10 +455,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>28.05566787719727</v>
+        <v>0.4596393704414368</v>
       </c>
       <c r="D6" t="n">
-        <v>88.3134663105011</v>
+        <v>0.7874612808227539</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -469,10 +469,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>26.72634720802307</v>
+        <v>0.4471473097801208</v>
       </c>
       <c r="D7" t="n">
-        <v>88.95891904830933</v>
+        <v>0.7941195964813232</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -483,10 +483,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>25.58122575283051</v>
+        <v>0.4223135411739349</v>
       </c>
       <c r="D8" t="n">
-        <v>89.54362273216248</v>
+        <v>0.8045355677604675</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -497,10 +497,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>24.7805193066597</v>
+        <v>0.4200760722160339</v>
       </c>
       <c r="D9" t="n">
-        <v>90.08277058601379</v>
+        <v>0.8075680732727051</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -511,10 +511,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>23.48838597536087</v>
+        <v>0.4121015965938568</v>
       </c>
       <c r="D10" t="n">
-        <v>90.51560759544373</v>
+        <v>0.8127101063728333</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -525,10 +525,290 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>22.30526506900787</v>
+        <v>0.3990113139152527</v>
       </c>
       <c r="D11" t="n">
-        <v>90.89528322219849</v>
+        <v>0.8204891681671143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.3999518156051636</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.8215439319610596</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.3939414024353027</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.8257630467414856</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.3930386304855347</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.824906051158905</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.3911015391349792</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.824114978313446</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.3888201713562012</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.8231920599937439</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.3787821233272552</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.8309051394462585</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>17</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.3797362744808197</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.8326850533485413</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>18</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.3773754239082336</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.8341354131698608</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>19</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.3776697814464569</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.8306414484977722</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.3735400140285492</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.8334102630615234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>21</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.3717670738697052</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.8351901769638062</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>22</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.3700553774833679</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.8362450003623962</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>23</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.368677020072937</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.839277446269989</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>24</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.3648383617401123</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.8412551879882812</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>25</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.3613282740116119</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.8415188789367676</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>26</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.3652969896793365</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.8402663469314575</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>27</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.3593234717845917</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.8412551879882812</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>28</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.3594219386577606</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.8403322696685791</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>29</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.3544694483280182</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.844880998134613</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>30</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.3567031621932983</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.842837393283844</v>
       </c>
     </row>
   </sheetData>

</xml_diff>